<commit_message>
Added os.getcwd() which returns current working directory of a process, created new directory xls, added a prints of start and ending of process
</commit_message>
<xml_diff>
--- a/xlsx/928.xlsx
+++ b/xlsx/928.xlsx
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="InputZip3">'[1]Intermediate Output'!$D$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3374,7 +3374,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J977"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A166" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A151" workbookViewId="0">
       <selection activeCell="H921" sqref="H921"/>
     </sheetView>
   </sheetViews>

</xml_diff>